<commit_message>
Mise à jour résultats avec marge 20%
</commit_message>
<xml_diff>
--- a/room_attribution/resultats/demi_journee_3/planning_presentateurs.xlsx
+++ b/room_attribution/resultats/demi_journee_3/planning_presentateurs.xlsx
@@ -466,22 +466,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>J007 (20 él.)</t>
+          <t>A101 (31 él.)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>D03 (87 él.)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>J021 (205 él.)</t>
+          <t>D03 (93 él.)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A115 (14 él.)</t>
         </is>
       </c>
     </row>
@@ -493,27 +493,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A116 (42 él.)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A017 (43 él.)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>I013 (65 él.)</t>
+          <t>J108 (38 él.)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>I013 (65 él.)</t>
+          <t>J108 (38 él.)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>J022 (86 él.)</t>
+          <t>J020 (56 él.)</t>
         </is>
       </c>
     </row>
@@ -525,27 +525,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>J106 (26 él.)</t>
+          <t>J009 (13 él.)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>D03 (102 él.)</t>
+          <t>J108 (38 él.)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>J107 (19 él.)</t>
+          <t>J020 (125 él.)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>J108 (40 él.)</t>
+          <t>J012 (24 él.)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>I013 (36 él.)</t>
+          <t>J110 (23 él.)</t>
         </is>
       </c>
     </row>
@@ -557,27 +557,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A017 (43 él.)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J109 (38 él.)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>J020 (117 él.)</t>
+          <t>A115 (45 él.)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>J022 (81 él.)</t>
+          <t>J110 (43 él.)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>J110 (6 él.)</t>
+          <t>D03 (35 él.)</t>
         </is>
       </c>
     </row>
@@ -589,27 +589,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J107 (13 él.)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>J021 (166 él.)</t>
+          <t>J107 (19 él.)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>J007 (20 él.)</t>
+          <t>J012 (24 él.)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J022 (155 él.)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>J012 (23 él.)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -621,27 +621,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>J204 (18 él.)</t>
+          <t>D03 (38 él.)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>J009 (20 él.)</t>
+          <t>D03 (96 él.)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>A016 (41 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>J020 (102 él.)</t>
+          <t>A016 (37 él.)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>A101 (23 él.)</t>
+          <t>J109 (33 él.)</t>
         </is>
       </c>
     </row>
@@ -653,27 +653,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>J109 (12 él.)</t>
+          <t>J110 (36 él.)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>J109 (38 él.)</t>
+          <t>I013 (60 él.)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>J021 (155 él.)</t>
+          <t>A012 (38 él.)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A116 (47 él.)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>D03 (6 él.)</t>
+          <t>J108 (30 él.)</t>
         </is>
       </c>
     </row>
@@ -685,27 +685,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>J020 (64 él.)</t>
+          <t>A012 (18 él.)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A101 (33 él.)</t>
+          <t>J020 (134 él.)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>J012 (26 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J106 (36 él.)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>J020 (89 él.)</t>
+          <t>J204 (24 él.)</t>
         </is>
       </c>
     </row>
@@ -717,27 +717,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A012 (25 él.)</t>
+          <t>A016 (19 él.)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>J020 (137 él.)</t>
+          <t>A016 (38 él.)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>A101 (33 él.)</t>
+          <t>I013 (60 él.)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>A101 (32 él.)</t>
+          <t>J020 (130 él.)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>J107 (20 él.)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -749,27 +749,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A017 (45 él.)</t>
+          <t>J108 (38 él.)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>I013 (61 él.)</t>
+          <t>A116 (48 él.)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>A017 (46 él.)</t>
+          <t>A013 (50 él.)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>J109 (41 él.)</t>
+          <t>I013 (60 él.)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>J021 (28 él.)</t>
+          <t>J022 (25 él.)</t>
         </is>
       </c>
     </row>
@@ -781,27 +781,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>J022 (31 él.)</t>
+          <t>J204 (20 él.)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>J022 (105 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>J110 (46 él.)</t>
+          <t>J106 (36 él.)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>A017 (39 él.)</t>
+          <t>J021 (148 él.)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J012 (17 él.)</t>
         </is>
       </c>
     </row>
@@ -813,27 +813,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A115 (47 él.)</t>
+          <t>J020 (45 él.)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>A017 (43 él.)</t>
+          <t>A012 (38 él.)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>A116 (52 él.)</t>
+          <t>A116 (47 él.)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>J110 (46 él.)</t>
+          <t>J109 (38 él.)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>A115 (20 él.)</t>
+          <t>A116 (41 él.)</t>
         </is>
       </c>
     </row>
@@ -845,27 +845,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>J108 (12 él.)</t>
+          <t>A013 (41 él.)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>J110 (42 él.)</t>
+          <t>A013 (50 él.)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>J022 (106 él.)</t>
+          <t>A017 (43 él.)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>J106 (39 él.)</t>
+          <t>A115 (45 él.)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>J009 (17 él.)</t>
+          <t>A017 (37 él.)</t>
         </is>
       </c>
     </row>
@@ -877,27 +877,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>I013 (50 él.)</t>
+          <t>A115 (45 él.)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>A116 (51 él.)</t>
+          <t>J106 (36 él.)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>A115 (49 él.)</t>
+          <t>A016 (38 él.)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>J008 (20 él.)</t>
+          <t>A013 (50 él.)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>J106 (28 él.)</t>
+          <t>A012 (29 él.)</t>
         </is>
       </c>
     </row>
@@ -909,27 +909,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A013 (47 él.)</t>
+          <t>J106 (12 él.)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>J204 (39 él.)</t>
+          <t>J022 (137 él.)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>A013 (53 él.)</t>
+          <t>A101 (31 él.)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>A116 (50 él.)</t>
+          <t>J204 (36 él.)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>A016 (35 él.)</t>
+          <t>J007 (9 él.)</t>
         </is>
       </c>
     </row>
@@ -941,27 +941,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>J110 (30 él.)</t>
+          <t>J022 (67 él.)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>A016 (40 él.)</t>
+          <t>J007 (19 él.)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>J204 (39 él.)</t>
+          <t>J110 (43 él.)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>D03 (102 él.)</t>
+          <t>A017 (43 él.)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>A017 (21 él.)</t>
+          <t>J021 (60 él.)</t>
         </is>
       </c>
     </row>
@@ -973,27 +973,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>A116 (44 él.)</t>
+          <t>I013 (33 él.)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>A115 (48 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>J108 (41 él.)</t>
+          <t>J022 (153 él.)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>A013 (54 él.)</t>
+          <t>J008 (19 él.)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>J109 (38 él.)</t>
+          <t>A013 (20 él.)</t>
         </is>
       </c>
     </row>
@@ -1005,27 +1005,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>A101 (17 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>J108 (39 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>D03 (98 él.)</t>
+          <t>J021 (169 él.)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>A115 (42 él.)</t>
+          <t>A012 (38 él.)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>A116 (11 él.)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1037,27 +1037,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>J021 (49 él.)</t>
+          <t>J007 (7 él.)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>A013 (52 él.)</t>
+          <t>J021 (152 él.)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>A012 (41 él.)</t>
+          <t>J109 (32 él.)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>J204 (39 él.)</t>
+          <t>J107 (18 él.)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>A012 (28 él.)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1069,27 +1069,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J109 (5 él.)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J008 (19 él.)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>J008 (18 él.)</t>
+          <t>J107 (17 él.)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>J009 (20 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>J204 (3 él.)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1101,17 +1101,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>J012 (7 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>J012 (26 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J204 (35 él.)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>A013 (7 él.)</t>
+          <t>J107 (5 él.)</t>
         </is>
       </c>
     </row>
@@ -1133,17 +1133,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>J009 (13 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J204 (34 él.)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>J109 (38 él.)</t>
+          <t>J008 (18 él.)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>J008 (11 él.)</t>
+          <t>J008 (15 él.)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1175,17 +1175,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J007 (18 él.)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>A016 (41 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A101 (19 él.)</t>
         </is>
       </c>
     </row>
@@ -1197,12 +1197,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>J107 (7 él.)</t>
+          <t>J012 (18 él.)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>J107 (13 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1212,12 +1212,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>J107 (19 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J106 (21 él.)</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A101 (6 él.)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1239,12 +1239,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>J009 (19 él.)</t>
+          <t>J009 (14 él.)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>J007 (19 él.)</t>
+          <t>J009 (18 él.)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A115 (45 él.)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1276,12 +1276,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>A012 (41 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>J007 (12 él.)</t>
+          <t>J009 (10 él.)</t>
         </is>
       </c>
     </row>
@@ -1293,12 +1293,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>A016 (12 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>A012 (38 él.)</t>
+          <t>J012 (24 él.)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A101 (26 él.)</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>J007 (7 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>J106 (28 él.)</t>
+          <t>J009 (19 él.)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A016 (16 él.)</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>J008 (20 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1372,12 +1372,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>J012 (24 él.)</t>
+          <t>J007 (19 él.)</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>I013 (22 él.)</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>D03 (23 él.)</t>
+          <t>J021 (23 él.)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>J108 (18 él.)</t>
+          <t>J008 (18 él.)</t>
         </is>
       </c>
     </row>
@@ -1426,12 +1426,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>J110 (43 él.)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>J106 (39 él.)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>J008 (9 él.)</t>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>